<commit_message>
Ignored blank lines when finding bigrams
The probability distributions for bigrams have been recomputed. This
time, the blank line at the end of the English words file was ignored.
</commit_message>
<xml_diff>
--- a/frequencies/bigrams.xlsx
+++ b/frequencies/bigrams.xlsx
@@ -2,12 +2,7 @@
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="17571"/>
-  <workbookPr defaultThemeVersion="166925"/>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-    <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\espli\Documents\GitHub\CS4783-Project-1\frequencies\"/>
-    </mc:Choice>
-  </mc:AlternateContent>
+  <workbookPr filterPrivacy="1" defaultThemeVersion="166925"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="19200" windowHeight="10200" activeTab="1"/>
   </bookViews>
@@ -15,7 +10,7 @@
     <sheet name="bigrams" sheetId="1" r:id="rId1"/>
     <sheet name="Probability" sheetId="3" r:id="rId2"/>
   </sheets>
-  <calcPr calcId="0"/>
+  <calcPr calcId="171027"/>
 </workbook>
 </file>
 
@@ -948,7 +943,7 @@
   <dimension ref="A1:AC28"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="H5" sqref="H5"/>
+      <selection activeCell="B2" sqref="B2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -1059,7 +1054,7 @@
         <v>27</v>
       </c>
       <c r="B2">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="C2">
         <v>6541</v>
@@ -1141,7 +1136,7 @@
       </c>
       <c r="AC2" s="1">
         <f t="shared" ref="AC2:AC28" si="0">SUM(B2:AB2)</f>
-        <v>109583</v>
+        <v>109582</v>
       </c>
     </row>
     <row r="3" spans="1:29" x14ac:dyDescent="0.35">
@@ -3486,6 +3481,7 @@
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
 
@@ -3594,111 +3590,111 @@
       </c>
       <c r="B2">
         <f>bigrams!B2/bigrams!$AC2</f>
-        <v>9.1255030433552654E-6</v>
+        <v>0</v>
       </c>
       <c r="C2">
         <f>bigrams!C2/bigrams!$AC2</f>
-        <v>5.9689915406586788E-2</v>
+        <v>5.9690460112062201E-2</v>
       </c>
       <c r="D2">
         <f>bigrams!D2/bigrams!$AC2</f>
-        <v>5.7308159112271065E-2</v>
+        <v>5.7308682082823824E-2</v>
       </c>
       <c r="E2">
         <f>bigrams!E2/bigrams!$AC2</f>
-        <v>9.4211693419599757E-2</v>
+        <v>9.4212553156540313E-2</v>
       </c>
       <c r="F2">
         <f>bigrams!F2/bigrams!$AC2</f>
-        <v>6.1086117372220146E-2</v>
+        <v>6.1086674818857115E-2</v>
       </c>
       <c r="G2">
         <f>bigrams!G2/bigrams!$AC2</f>
-        <v>4.1010010676838564E-2</v>
+        <v>4.1010384917230934E-2</v>
       </c>
       <c r="H2">
         <f>bigrams!H2/bigrams!$AC2</f>
-        <v>4.2898989806813101E-2</v>
+        <v>4.2899381285247576E-2</v>
       </c>
       <c r="I2">
         <f>bigrams!I2/bigrams!$AC2</f>
-        <v>3.279705793781882E-2</v>
+        <v>3.2797357230202037E-2</v>
       </c>
       <c r="J2">
         <f>bigrams!J2/bigrams!$AC2</f>
-        <v>3.5771971929952635E-2</v>
+        <v>3.5772298370170284E-2</v>
       </c>
       <c r="K2">
         <f>bigrams!K2/bigrams!$AC2</f>
-        <v>3.9987954335982769E-2</v>
+        <v>3.9988319249511781E-2</v>
       </c>
       <c r="L2">
         <f>bigrams!L2/bigrams!$AC2</f>
-        <v>9.5452761833496064E-3</v>
+        <v>9.5453632895913555E-3</v>
       </c>
       <c r="M2">
         <f>bigrams!M2/bigrams!$AC2</f>
-        <v>8.7969849337944748E-3</v>
+        <v>8.7970652114398359E-3</v>
       </c>
       <c r="N2">
         <f>bigrams!N2/bigrams!$AC2</f>
-        <v>3.0689066734803757E-2</v>
+        <v>3.0689346790531292E-2</v>
       </c>
       <c r="O2">
         <f>bigrams!O2/bigrams!$AC2</f>
-        <v>5.298267066972067E-2</v>
+        <v>5.2983154167655269E-2</v>
       </c>
       <c r="P2">
         <f>bigrams!P2/bigrams!$AC2</f>
-        <v>2.2585620032304281E-2</v>
+        <v>2.2585826139329451E-2</v>
       </c>
       <c r="Q2">
         <f>bigrams!Q2/bigrams!$AC2</f>
-        <v>2.7066242026591716E-2</v>
+        <v>2.706648902191966E-2</v>
       </c>
       <c r="R2">
         <f>bigrams!R2/bigrams!$AC2</f>
-        <v>7.7092249710265279E-2</v>
+        <v>7.7092953222244534E-2</v>
       </c>
       <c r="S2">
         <f>bigrams!S2/bigrams!$AC2</f>
-        <v>5.2654152560159878E-3</v>
+        <v>5.2654633060174117E-3</v>
       </c>
       <c r="T2">
         <f>bigrams!T2/bigrams!$AC2</f>
-        <v>6.2089922706989223E-2</v>
+        <v>6.2090489313938423E-2</v>
       </c>
       <c r="U2">
         <f>bigrams!U2/bigrams!$AC2</f>
-        <v>0.11049159084894555</v>
+        <v>0.11049259914949536</v>
       </c>
       <c r="V2">
         <f>bigrams!V2/bigrams!$AC2</f>
-        <v>5.0464031829754619E-2</v>
+        <v>5.046449234363308E-2</v>
       </c>
       <c r="W2">
         <f>bigrams!W2/bigrams!$AC2</f>
-        <v>3.0223666079592638E-2</v>
+        <v>3.0223941888266322E-2</v>
       </c>
       <c r="X2">
         <f>bigrams!X2/bigrams!$AC2</f>
-        <v>1.6654043054123359E-2</v>
+        <v>1.6654195032030809E-2</v>
       </c>
       <c r="Y2">
         <f>bigrams!Y2/bigrams!$AC2</f>
-        <v>2.476661525966619E-2</v>
+        <v>2.476684126955157E-2</v>
       </c>
       <c r="Z2">
         <f>bigrams!Z2/bigrams!$AC2</f>
-        <v>7.2091474042506589E-4</v>
+        <v>7.2092131919475832E-4</v>
       </c>
       <c r="AA2">
         <f>bigrams!AA2/bigrams!$AC2</f>
-        <v>3.3764361260414481E-3</v>
+        <v>3.3764669380007667E-3</v>
       </c>
       <c r="AB2">
         <f>bigrams!AB2/bigrams!$AC2</f>
-        <v>2.4182583064891452E-3</v>
+        <v>2.4182803745140626E-3</v>
       </c>
     </row>
     <row r="3" spans="1:28" x14ac:dyDescent="0.35">
@@ -6641,5 +6637,6 @@
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>